<commit_message>
PCB update with changes from Greg comments
</commit_message>
<xml_diff>
--- a/Project Prototype/PCB_Autobot/Autobot_project/Project Outputs for Autobot_project/BOM/Bill of Materials-Autobot_project.xlsx
+++ b/Project Prototype/PCB_Autobot/Autobot_project/Project Outputs for Autobot_project/BOM/Bill of Materials-Autobot_project.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="112">
   <si>
     <t>Comment</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Motor, General Kind</t>
   </si>
   <si>
-    <t>RB5-10.5</t>
+    <t>BORNIER</t>
   </si>
   <si>
     <t>Olimex</t>
@@ -120,13 +120,13 @@
     <t>Cap</t>
   </si>
   <si>
-    <t>C1, C1, C1, C3, C3, C3, C5, C5, C5, C11</t>
+    <t>C1, C1, C1, C2, C2, C2, C3, C3, C3, C5, C5, C5, C11, C16, C17, C18, C18, C18</t>
   </si>
   <si>
     <t>220uF</t>
   </si>
   <si>
-    <t>C2, C2, C2, C4, C4, C4</t>
+    <t>C4</t>
   </si>
   <si>
     <t>100nF</t>
@@ -135,7 +135,7 @@
     <t>C6, C7</t>
   </si>
   <si>
-    <t>C8, C9, C15</t>
+    <t>C8, C9</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -147,7 +147,7 @@
     <t>22uF</t>
   </si>
   <si>
-    <t>C16, C17</t>
+    <t>C15</t>
   </si>
   <si>
     <t>Diode</t>
@@ -198,21 +198,18 @@
     <t>6-pin Connector</t>
   </si>
   <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>22-11-2062</t>
+  </si>
+  <si>
+    <t>1462951</t>
+  </si>
+  <si>
     <t>ICSP</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>0402-A</t>
-  </si>
-  <si>
-    <t>3.3uH</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
     <t>L298N</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>Microphone</t>
   </si>
   <si>
-    <t>PIN2</t>
-  </si>
-  <si>
     <t>Mic2</t>
   </si>
   <si>
@@ -252,6 +246,15 @@
     <t>44TQFP</t>
   </si>
   <si>
+    <t>MICROCHIP</t>
+  </si>
+  <si>
+    <t>PIC32MX250F128D-50I-PT</t>
+  </si>
+  <si>
+    <t>2357347</t>
+  </si>
+  <si>
     <t>PIC</t>
   </si>
   <si>
@@ -267,7 +270,7 @@
     <t>Res1</t>
   </si>
   <si>
-    <t>R1, R1, R1, R3, R13</t>
+    <t>R1, R1, R1, R3</t>
   </si>
   <si>
     <t>10R</t>
@@ -282,6 +285,12 @@
     <t>R4</t>
   </si>
   <si>
+    <t>820R</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
     <t>330R</t>
   </si>
   <si>
@@ -294,10 +303,10 @@
     <t>R8, R10</t>
   </si>
   <si>
-    <t>33.2KR</t>
-  </si>
-  <si>
-    <t>R12</t>
+    <t>1000R</t>
+  </si>
+  <si>
+    <t>R14</t>
   </si>
   <si>
     <t>SW-PB</t>
@@ -309,13 +318,13 @@
     <t>SPST-2</t>
   </si>
   <si>
-    <t>[NoValue], MULTICOMP, [NoValue]</t>
-  </si>
-  <si>
-    <t>[NoValue], R13-509B-05-BR, [NoValue]</t>
-  </si>
-  <si>
-    <t>[NoValue], 1634685, [NoValue]</t>
+    <t>[NoValue], MULTICOMP, MULTICOMP</t>
+  </si>
+  <si>
+    <t>[NoValue], R13-509B-05-BR, R13-608C1-02-BB-9A</t>
+  </si>
+  <si>
+    <t>[NoValue], 1634685, 1634617</t>
   </si>
   <si>
     <t>S1, S2, S3</t>
@@ -324,9 +333,6 @@
     <t>FT232R</t>
   </si>
   <si>
-    <t>MOLEX</t>
-  </si>
-  <si>
     <t>22-27-2041</t>
   </si>
   <si>
@@ -336,10 +342,16 @@
     <t>UART</t>
   </si>
   <si>
-    <t>TPS562200</t>
-  </si>
-  <si>
-    <t>VReg</t>
+    <t>LM1117SX-3.3</t>
+  </si>
+  <si>
+    <t>TO-263-3</t>
+  </si>
+  <si>
+    <t>LM1117SX-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>2323594</t>
   </si>
   <si>
     <t>V Reg</t>
@@ -830,7 +842,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>12</v>
@@ -856,7 +868,7 @@
         <v>32</v>
       </c>
       <c r="E5" s="3">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>29</v>
@@ -891,7 +903,7 @@
         <v>32</v>
       </c>
       <c r="E6" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>34</v>
@@ -961,7 +973,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>36</v>
@@ -1031,7 +1043,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>41</v>
@@ -1177,51 +1189,51 @@
         <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>63</v>
@@ -1229,92 +1241,92 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E16" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>12</v>
@@ -1329,27 +1341,27 @@
         <v>12</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>12</v>
@@ -1364,27 +1376,27 @@
         <v>12</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>12</v>
@@ -1399,27 +1411,27 @@
         <v>12</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>12</v>
@@ -1434,27 +1446,27 @@
         <v>12</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E22" s="3">
         <v>4</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>12</v>
@@ -1469,27 +1481,27 @@
         <v>12</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E23" s="3">
         <v>2</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>12</v>
@@ -1504,27 +1516,27 @@
         <v>12</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E24" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>12</v>
@@ -1539,21 +1551,21 @@
         <v>12</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E25" s="3">
         <v>3</v>
@@ -1562,24 +1574,24 @@
         <v>12</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
@@ -1588,7 +1600,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1597,33 +1609,33 @@
         <v>12</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
@@ -1632,19 +1644,19 @@
         <v>12</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resistances / condensateurs update based on MIC POC working
</commit_message>
<xml_diff>
--- a/Project Prototype/PCB_Autobot/Autobot_project/Project Outputs for Autobot_project/BOM/Bill of Materials-Autobot_project.xlsx
+++ b/Project Prototype/PCB_Autobot/Autobot_project/Project Outputs for Autobot_project/BOM/Bill of Materials-Autobot_project.xlsx
@@ -108,22 +108,28 @@
     <t>BT1</t>
   </si>
   <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>CAPC1608N</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>C1, C1, C1, C3, C3, C3, C5, C5, C5, C10, C12, C13, C14</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>CAPC1608N</t>
-  </si>
-  <si>
-    <t>Cap</t>
-  </si>
-  <si>
-    <t>C1, C1, C1, C2, C2, C2, C3, C3, C3, C5, C5, C5, C11, C16, C17, C18, C18, C18</t>
-  </si>
-  <si>
-    <t>220uF</t>
+    <t>C2, C2, C2, C11, C16, C17, C18, C18, C18</t>
+  </si>
+  <si>
+    <t>47pF</t>
   </si>
   <si>
     <t>C4</t>
@@ -138,12 +144,6 @@
     <t>C8, C9</t>
   </si>
   <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>C10, C12, C13, C14</t>
-  </si>
-  <si>
     <t>22uF</t>
   </si>
   <si>
@@ -258,25 +258,31 @@
     <t>PIC</t>
   </si>
   <si>
+    <t>330R</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>RESC1608N</t>
+  </si>
+  <si>
+    <t>Res1</t>
+  </si>
+  <si>
+    <t>R1, R1, R1, R6, R7, R9, R11</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
     <t>10KR</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>RESC1608N</t>
-  </si>
-  <si>
-    <t>Res1</t>
-  </si>
-  <si>
-    <t>R1, R1, R1, R3</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R2</t>
+    <t>R3</t>
   </si>
   <si>
     <t>1KR</t>
@@ -285,25 +291,19 @@
     <t>R4</t>
   </si>
   <si>
-    <t>820R</t>
+    <t>360KR</t>
   </si>
   <si>
     <t>R5</t>
   </si>
   <si>
-    <t>330R</t>
-  </si>
-  <si>
-    <t>R6, R7, R9, R11</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
     <t>R8, R10</t>
   </si>
   <si>
-    <t>1000R</t>
+    <t>430KR</t>
   </si>
   <si>
     <t>R14</t>
@@ -868,7 +868,7 @@
         <v>32</v>
       </c>
       <c r="E5" s="3">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>29</v>
@@ -903,7 +903,7 @@
         <v>32</v>
       </c>
       <c r="E6" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>34</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
@@ -938,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>36</v>
@@ -961,7 +961,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>30</v>
@@ -976,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>12</v>
@@ -991,12 +991,12 @@
         <v>12</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>30</v>
@@ -1008,10 +1008,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>12</v>
@@ -1323,7 +1323,7 @@
         <v>82</v>
       </c>
       <c r="E18" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>79</v>
@@ -1428,7 +1428,7 @@
         <v>82</v>
       </c>
       <c r="E21" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>88</v>
@@ -1463,7 +1463,7 @@
         <v>82</v>
       </c>
       <c r="E22" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>90</v>

</xml_diff>